<commit_message>
add word for milestone 1
milestone 1 created word and sheered it
</commit_message>
<xml_diff>
--- a/EEE3099s.xlsx
+++ b/EEE3099s.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uctcloud-my.sharepoint.com/personal/frskia001_myuct_ac_za/Documents/Desktop/uct/3 year/second semester/99/EEE3099S_CKT/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="23" documentId="8_{CB3CCE28-6622-4C81-9BD5-968F7B7D27BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E7E8B3B1-A01A-4676-8A95-D77528D9E4AF}"/>
+  <xr:revisionPtr revIDLastSave="28" documentId="8_{CB3CCE28-6622-4C81-9BD5-968F7B7D27BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FDFDBB5B-CCEA-441A-B042-7B95C7FD8794}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="15540" yWindow="1524" windowWidth="7500" windowHeight="6000" xr2:uid="{67C68725-19BE-4398-ACF2-00E343F90CD0}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{67C68725-19BE-4398-ACF2-00E343F90CD0}"/>
   </bookViews>
   <sheets>
     <sheet name="contribution" sheetId="1" r:id="rId1"/>
@@ -36,10 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
-  <si>
-    <t>contributions</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t xml:space="preserve">who did it </t>
   </si>
@@ -51,6 +48,12 @@
   </si>
   <si>
     <t>cotibution excel</t>
+  </si>
+  <si>
+    <t>contributions for we move</t>
+  </si>
+  <si>
+    <t xml:space="preserve">kian </t>
   </si>
 </sst>
 </file>
@@ -520,18 +523,14 @@
   <dimension ref="A1:D25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4:D5"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="9.44140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.6640625" bestFit="1" customWidth="1"/>
-  </cols>
+  <sheetFormatPr defaultColWidth="19.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:4" ht="23.4" x14ac:dyDescent="0.45">
       <c r="A1" s="4" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="B1" s="5"/>
       <c r="C1" s="1"/>
@@ -539,22 +538,24 @@
     </row>
     <row r="2" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="7" t="s">
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3" s="3" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A3" s="3" t="s">
+      <c r="B3" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="3" t="s">
-        <v>4</v>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4" s="2" t="s">
+        <v>5</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A4" s="2"/>
       <c r="B4" s="2"/>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Fixed spelling errors on Timeline
</commit_message>
<xml_diff>
--- a/EEE3099s.xlsx
+++ b/EEE3099s.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pilla\Desktop\EEE3099S_WeMove\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{100B0BC2-5D34-42CD-8AA8-89366C6A2798}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{214BF014-E348-4D70-9DBF-4CD416F71503}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4860" yWindow="3420" windowWidth="21600" windowHeight="11295" xr2:uid="{67C68725-19BE-4398-ACF2-00E343F90CD0}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{67C68725-19BE-4398-ACF2-00E343F90CD0}"/>
   </bookViews>
   <sheets>
     <sheet name="contribution" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <t xml:space="preserve">who did it </t>
   </si>
@@ -48,9 +48,6 @@
   </si>
   <si>
     <t>contributions for we move</t>
-  </si>
-  <si>
-    <t xml:space="preserve">kian </t>
   </si>
   <si>
     <t>contribution excel</t>
@@ -522,7 +519,7 @@
   <dimension ref="A1:B25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="19.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -546,13 +543,11 @@
         <v>2</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
         <v>4</v>
       </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="1"/>
       <c r="B4" s="1"/>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">

</xml_diff>